<commit_message>
Added script for gcash and MPIN
</commit_message>
<xml_diff>
--- a/src/test/resources/com/multisys/excel/testdata.xlsx
+++ b/src/test/resources/com/multisys/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>TCID</t>
   </si>
@@ -136,18 +136,9 @@
     <t>Daniella Columbres</t>
   </si>
   <si>
-    <t>5105105105105100</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>052021</t>
-  </si>
-  <si>
-    <t>776</t>
-  </si>
-  <si>
     <t>PayThruCash</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>PayThruVisa</t>
   </si>
   <si>
-    <t>9610596387</t>
-  </si>
-  <si>
     <t>Payment Method</t>
   </si>
   <si>
@@ -200,6 +188,30 @@
   </si>
   <si>
     <t>PayThruMasterCard</t>
+  </si>
+  <si>
+    <t>9165523448</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>MPIN</t>
+  </si>
+  <si>
+    <t>888888</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>4444333322221111</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>122025</t>
   </si>
 </sst>
 </file>
@@ -537,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,31 +568,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -588,7 +600,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -596,7 +608,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -604,7 +616,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -612,7 +624,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -620,7 +632,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -628,23 +640,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>3</v>
@@ -660,7 +672,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,21 +685,21 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -699,12 +711,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
     <col min="3" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" customWidth="1"/>
     <col min="6" max="12" width="17.6328125" customWidth="1"/>
@@ -802,23 +816,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +860,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,16 +886,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +909,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -907,16 +936,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added script for gcash OTP and MPIN
</commit_message>
<xml_diff>
--- a/src/test/resources/com/multisys/excel/testdata.xlsx
+++ b/src/test/resources/com/multisys/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>TCID</t>
   </si>
@@ -151,22 +151,7 @@
     <t>PayThruVisa</t>
   </si>
   <si>
-    <t>Payment Method</t>
-  </si>
-  <si>
-    <t>E-Wallet</t>
-  </si>
-  <si>
-    <t>Gcash</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>HappyPath</t>
-  </si>
-  <si>
-    <t>E-wallets</t>
   </si>
   <si>
     <t>PayThruAllEasy</t>
@@ -547,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +556,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -592,7 +577,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -600,7 +585,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -608,7 +593,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -616,7 +601,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -624,7 +609,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -632,7 +617,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -640,7 +625,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
@@ -651,14 +636,6 @@
         <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -669,37 +646,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -818,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,21 +795,21 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +822,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -886,16 +848,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -909,7 +871,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +879,7 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -936,16 +898,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added script for cash payment
</commit_message>
<xml_diff>
--- a/src/test/resources/com/multisys/excel/testdata.xlsx
+++ b/src/test/resources/com/multisys/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>TCID</t>
   </si>
@@ -166,9 +166,6 @@
     <t>PayThruGrabPH</t>
   </si>
   <si>
-    <t>PayThruUnionBank</t>
-  </si>
-  <si>
     <t>PayThruWeChatPay</t>
   </si>
   <si>
@@ -197,6 +194,15 @@
   </si>
   <si>
     <t>122025</t>
+  </si>
+  <si>
+    <t>Reference Number</t>
+  </si>
+  <si>
+    <t>PayThruUnionPay</t>
+  </si>
+  <si>
+    <t>MarkPaymentAsPaid</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,20 +562,20 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -577,7 +583,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -585,7 +591,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -593,7 +599,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -601,15 +607,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -617,7 +623,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -625,7 +631,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
@@ -633,9 +639,17 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -648,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" activeCellId="1" sqref="E11 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,10 +685,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +700,7 @@
     <col min="6" max="12" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -726,8 +740,11 @@
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -795,21 +812,21 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -848,16 +865,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -898,16 +915,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added script for cash payments
</commit_message>
<xml_diff>
--- a/src/test/resources/com/multisys/excel/testdata.xlsx
+++ b/src/test/resources/com/multisys/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>TCID</t>
   </si>
@@ -157,52 +157,49 @@
     <t>PayThruAllEasy</t>
   </si>
   <si>
+    <t>PayThruCoinsPH</t>
+  </si>
+  <si>
+    <t>PayThruGrabPH</t>
+  </si>
+  <si>
+    <t>PayThruWeChatPay</t>
+  </si>
+  <si>
+    <t>PayThruMasterCard</t>
+  </si>
+  <si>
+    <t>9165523448</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>MPIN</t>
+  </si>
+  <si>
+    <t>888888</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>4444333322221111</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>122025</t>
+  </si>
+  <si>
+    <t>PayThruUnionPay</t>
+  </si>
+  <si>
+    <t>MarkPaymentAsPaid</t>
+  </si>
+  <si>
     <t>PayThruAliPay</t>
-  </si>
-  <si>
-    <t>PayThruCoinsPH</t>
-  </si>
-  <si>
-    <t>PayThruGrabPH</t>
-  </si>
-  <si>
-    <t>PayThruWeChatPay</t>
-  </si>
-  <si>
-    <t>PayThruMasterCard</t>
-  </si>
-  <si>
-    <t>9165523448</t>
-  </si>
-  <si>
-    <t>OTP</t>
-  </si>
-  <si>
-    <t>MPIN</t>
-  </si>
-  <si>
-    <t>888888</t>
-  </si>
-  <si>
-    <t>11111</t>
-  </si>
-  <si>
-    <t>4444333322221111</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>122025</t>
-  </si>
-  <si>
-    <t>Reference Number</t>
-  </si>
-  <si>
-    <t>PayThruUnionPay</t>
-  </si>
-  <si>
-    <t>MarkPaymentAsPaid</t>
   </si>
 </sst>
 </file>
@@ -540,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,15 +559,15 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -591,7 +588,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -607,15 +604,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -623,7 +620,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -631,7 +628,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
@@ -639,7 +636,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
@@ -662,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" activeCellId="1" sqref="E11 E17"/>
     </sheetView>
   </sheetViews>
@@ -685,10 +682,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,7 +697,7 @@
     <col min="6" max="12" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -740,11 +737,8 @@
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -782,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -812,21 +806,21 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -865,16 +859,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -915,16 +909,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>